<commit_message>
Modified Result Task TuTM, ThiVT
</commit_message>
<xml_diff>
--- a/Document/Tasks/Task7-1.xlsx
+++ b/Document/Tasks/Task7-1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
   <si>
     <t>Project Code:</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Trên Source3 chưa thấy đường dẫn tới form của DungDV</t>
+  </si>
+  <si>
+    <t>Thiếu nhiều Bảng</t>
   </si>
 </sst>
 </file>
@@ -635,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="C7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -738,10 +741,10 @@
       <c r="H5" s="12">
         <v>3</v>
       </c>
-      <c r="I5" s="12">
-        <v>2</v>
-      </c>
-      <c r="J5" s="12">
+      <c r="I5" s="20">
+        <v>2</v>
+      </c>
+      <c r="J5" s="20">
         <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -770,10 +773,10 @@
       <c r="H6" s="12">
         <v>3</v>
       </c>
-      <c r="I6" s="12">
-        <v>2</v>
-      </c>
-      <c r="J6" s="12">
+      <c r="I6" s="20">
+        <v>2</v>
+      </c>
+      <c r="J6" s="20">
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -988,14 +991,19 @@
       <c r="H12" s="12">
         <v>3</v>
       </c>
-      <c r="I12" s="12">
-        <v>2</v>
-      </c>
-      <c r="J12" s="12">
+      <c r="I12" s="20">
+        <v>2</v>
+      </c>
+      <c r="J12" s="20">
         <v>2</v>
       </c>
       <c r="K12" s="12"/>
-      <c r="P12" s="14"/>
+      <c r="N12" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B13" s="17">
@@ -1027,10 +1035,10 @@
       </c>
       <c r="K13" s="4"/>
       <c r="N13" t="s">
-        <v>33</v>
-      </c>
-      <c r="P13" s="14">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="P13" s="9">
+        <v>3.5</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
@@ -1063,10 +1071,10 @@
       </c>
       <c r="K14" s="4"/>
       <c r="N14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P14" s="9">
-        <v>3.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.2">
@@ -1099,10 +1107,10 @@
       </c>
       <c r="K15" s="4"/>
       <c r="N15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P15" s="9">
-        <v>4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.2">
@@ -1135,10 +1143,10 @@
       </c>
       <c r="K16" s="4"/>
       <c r="N16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="P16" s="9">
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
@@ -1161,7 +1169,7 @@
         <v>3.5</v>
       </c>
       <c r="H17" s="12">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="I17" s="12">
         <v>3.5</v>
@@ -1171,10 +1179,7 @@
       </c>
       <c r="K17" s="4"/>
       <c r="N17" t="s">
-        <v>14</v>
-      </c>
-      <c r="P17" s="9">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
@@ -1194,7 +1199,7 @@
         <v>6</v>
       </c>
       <c r="G18" s="12">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H18" s="12">
         <v>3.5</v>
@@ -1207,7 +1212,7 @@
       </c>
       <c r="K18" s="4"/>
       <c r="N18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P18" s="9"/>
     </row>
@@ -1227,13 +1232,21 @@
       <c r="F19" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
+      <c r="G19" s="20">
+        <v>2</v>
+      </c>
+      <c r="H19" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="I19" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="J19" s="12">
+        <v>3.5</v>
+      </c>
       <c r="K19" s="4"/>
-      <c r="N19" t="s">
-        <v>18</v>
+      <c r="N19" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:16" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -1256,7 +1269,7 @@
         <v>3.5</v>
       </c>
       <c r="H20" s="12">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="I20" s="12">
         <v>3.5</v>
@@ -1266,7 +1279,7 @@
       </c>
       <c r="K20" s="12"/>
       <c r="N20" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:16" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -1292,14 +1305,14 @@
         <v>3</v>
       </c>
       <c r="I21" s="12">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="J21" s="12">
         <v>3.5</v>
       </c>
       <c r="K21" s="12"/>
       <c r="N21" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:16" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -1318,8 +1331,8 @@
       <c r="F22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="12">
-        <v>3</v>
+      <c r="G22" s="20">
+        <v>2</v>
       </c>
       <c r="H22" s="12">
         <v>3.5</v>
@@ -1331,9 +1344,6 @@
         <v>3.5</v>
       </c>
       <c r="K22" s="12"/>
-      <c r="N22" s="10" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23" s="17">
@@ -1349,13 +1359,23 @@
         <v>3</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="G23" s="20">
+        <v>2</v>
+      </c>
+      <c r="H23" s="20">
+        <v>2</v>
+      </c>
+      <c r="I23" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="J23" s="12">
+        <v>3</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="24" spans="2:16" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="17">
@@ -1759,14 +1779,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F27:F55 D27:D55 E26:E55">
       <formula1>$U$7:$U$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D26">
-      <formula1>$N$7:$N$20</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F26">
       <formula1>$O$7:$O$8</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D26">
+      <formula1>$N$7:$N$19</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:J55">
-      <formula1>$P$7:$P$17</formula1>
+      <formula1>$P$7:$P$16</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>